<commit_message>
Phao thi bac 5
</commit_message>
<xml_diff>
--- a/20210517/Phaothi.xlsx
+++ b/20210517/Phaothi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03_Tools\03_linhtinh\GitHub\NhungLe\20210517\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16C0FF5-F1DB-4F14-8B9C-A87BC5251776}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7521FB63-0A2F-45E8-9625-751649E8A49E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B53A822-AC92-4326-B772-AFD194ECEA34}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>IRR</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>293.9/((1+IRR)^4)</t>
+  </si>
+  <si>
+    <t>293.9/((1+IRR)^5)</t>
   </si>
 </sst>
 </file>
@@ -467,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BACCD38-0107-4555-BE39-9902B1432C35}">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J100" sqref="J100"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,10 +483,12 @@
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
@@ -500,10 +505,13 @@
         <v>293.89999999999998</v>
       </c>
       <c r="H1" s="2">
-        <v>-430</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>293.89999999999998</v>
+      </c>
+      <c r="I1" s="2">
+        <v>-430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -525,16 +533,19 @@
       <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="7">
-        <v>-430</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="7">
+        <v>-430</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="str">
-        <f>IF(AND(0&lt;I3,I3*I4&lt;0),"Co the la nghiem","-")</f>
+        <f>IF(AND(0&lt;J3,J3*J4&lt;0),"Co the la nghiem","-")</f>
         <v>-</v>
       </c>
       <c r="B3" s="3">
@@ -561,17 +572,21 @@
         <v>293.89999999999998</v>
       </c>
       <c r="H3" s="3">
-        <f>$H$1</f>
-        <v>-430</v>
-      </c>
-      <c r="I3" s="4">
-        <f>SUM(D3:H3)</f>
-        <v>469.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <f>$H$1/(C3^5)</f>
+        <v>293.89999999999998</v>
+      </c>
+      <c r="I3" s="3">
+        <f>$I$1</f>
+        <v>-430</v>
+      </c>
+      <c r="J3" s="4">
+        <f>SUM(D3:I3)</f>
+        <v>763.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
-        <f t="shared" ref="A4:A67" si="0">IF(AND(0&lt;I4,I4*I5&lt;0),"Co the la nghiem","-")</f>
+        <f t="shared" ref="A4:A67" si="0">IF(AND(0&lt;J4,J4*J5&lt;0),"Co the la nghiem","-")</f>
         <v>-</v>
       </c>
       <c r="B4" s="3">
@@ -598,15 +613,19 @@
         <v>282.43212324349969</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H67" si="6">$H$1</f>
-        <v>-430</v>
-      </c>
-      <c r="I4" s="4">
-        <f t="shared" ref="I4:I67" si="7">SUM(D4:H4)</f>
-        <v>446.21703658435831</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H4:H67" si="6">$H$1/(C4^5)</f>
+        <v>279.6357655876235</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I67" si="7">$I$1</f>
+        <v>-430</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" ref="J4:J67" si="8">SUM(D4:I4)</f>
+        <v>725.85280217198169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -636,14 +655,18 @@
       </c>
       <c r="H5" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I5" s="4">
-        <f t="shared" si="7"/>
-        <v>423.77420345677831</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>266.19428500901228</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="8"/>
+        <v>689.96848846579064</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -673,14 +696,18 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I6" s="4">
-        <f t="shared" si="7"/>
-        <v>402.22297593565702</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>253.52072173050581</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="8"/>
+        <v>655.74369766616292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -710,14 +737,18 @@
       </c>
       <c r="H7" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="7"/>
-        <v>381.51783135219353</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>241.5643766765734</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="8"/>
+        <v>623.0822080287669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -747,14 +778,18 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="7"/>
-        <v>361.61603447123366</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>230.27834032508008</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="8"/>
+        <v>591.89437479631374</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -784,14 +819,18 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="7"/>
-        <v>342.47744022195843</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>219.61917700533411</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" si="8"/>
+        <v>562.09661722729254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -821,14 +860,18 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="7"/>
-        <v>324.06431218843875</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>209.54663815025012</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="8"/>
+        <v>533.61095033868889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -858,14 +901,18 @@
       </c>
       <c r="H11" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="7"/>
-        <v>306.34115546222426</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>200.02340160821998</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="8"/>
+        <v>506.36455707044422</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -895,14 +942,18 @@
       </c>
       <c r="H12" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="7"/>
-        <v>289.27456259507358</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>191.01483443308365</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="8"/>
+        <v>480.28939702815728</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -932,14 +983,18 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="7"/>
-        <v>272.83307151150871</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>182.48877684708563</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="8"/>
+        <v>455.32184835859437</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -969,14 +1024,18 @@
       </c>
       <c r="H14" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="7"/>
-        <v>256.98703434974391</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>174.41534531641037</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="8"/>
+        <v>431.40237966615427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1006,14 +1065,18 @@
       </c>
       <c r="H15" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="7"/>
-        <v>241.70849629711574</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>166.7667528956963</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="8"/>
+        <v>408.47524919281204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1043,14 +1106,18 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="7"/>
-        <v>226.97108357368643</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159.51714519023793</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="8"/>
+        <v>386.48822876392433</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1080,14 +1147,18 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="7"/>
-        <v>212.74989979633369</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>152.64245045534969</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="8"/>
+        <v>365.39235025168341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1117,14 +1188,18 @@
       </c>
       <c r="H18" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="7"/>
-        <v>199.02143002633659</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146.12024250416738</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="8"/>
+        <v>345.14167253050391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1154,14 +1229,18 @@
       </c>
       <c r="H19" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="7"/>
-        <v>185.76345186707977</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>139.92961523023408</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="8"/>
+        <v>325.69306709731381</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1191,14 +1270,18 @@
       </c>
       <c r="H20" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="7"/>
-        <v>172.95495303583402</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>134.05106767156028</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="8"/>
+        <v>307.00602070739433</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1228,14 +1311,18 @@
       </c>
       <c r="H21" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="7"/>
-        <v>160.57605488521813</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>128.46639865013179</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="8"/>
+        <v>289.04245353534998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1265,14 +1352,18 @@
       </c>
       <c r="H22" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I22" s="4">
-        <f t="shared" si="7"/>
-        <v>148.60794139660788</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>123.15861011662281</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="8"/>
+        <v>271.76655151323075</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1302,14 +1393,18 @@
       </c>
       <c r="H23" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="7"/>
-        <v>137.03279320987656</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>118.11181841563786</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="8"/>
+        <v>255.14461162551447</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1339,14 +1434,18 @@
       </c>
       <c r="H24" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I24" s="4">
-        <f t="shared" si="7"/>
-        <v>125.83372629193752</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>113.31117276333939</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="8"/>
+        <v>239.14489905527694</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1376,14 +1475,18 @@
       </c>
       <c r="H25" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I25" s="4">
-        <f t="shared" si="7"/>
-        <v>114.99473488103752</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>108.74278029782658</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="8"/>
+        <v>223.7375151788641</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1413,14 +1516,18 @@
       </c>
       <c r="H26" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I26" s="4">
-        <f t="shared" si="7"/>
-        <v>104.50063837495873</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>104.39363712401823</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" si="8"/>
+        <v>208.89427549897698</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1450,14 +1557,18 @@
       </c>
       <c r="H27" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I27" s="4">
-        <f t="shared" si="7"/>
-        <v>94.337031859589501</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100.25156482984772</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="8"/>
+        <v>194.58859668943728</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1487,14 +1598,18 @@
       </c>
       <c r="H28" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I28" s="4">
-        <f t="shared" si="7"/>
-        <v>84.490239999999972</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96.305151999999993</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="8"/>
+        <v>180.79539199999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1524,14 +1639,18 @@
       </c>
       <c r="H29" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I29" s="4">
-        <f t="shared" si="7"/>
-        <v>74.947274039464673</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>92.543700297823463</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" si="8"/>
+        <v>167.49097433728809</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1561,14 +1680,18 @@
       </c>
       <c r="H30" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I30" s="4">
-        <f t="shared" si="7"/>
-        <v>65.695791673063923</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>88.957174725980877</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" si="8"/>
+        <v>154.65296639904477</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1598,14 +1721,18 @@
       </c>
       <c r="H31" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I31" s="4">
-        <f t="shared" si="7"/>
-        <v>56.724059581756592</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>85.536157712340341</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" si="8"/>
+        <v>142.26021729409695</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1635,14 +1762,18 @@
       </c>
       <c r="H32" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I32" s="4">
-        <f t="shared" si="7"/>
-        <v>48.020918430355266</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>82.271806699981937</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J32" s="4">
+        <f t="shared" si="8"/>
+        <v>130.2927251303372</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1672,14 +1803,18 @@
       </c>
       <c r="H33" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I33" s="4">
-        <f t="shared" si="7"/>
-        <v>39.575750148804275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79.155814949379575</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J33" s="4">
+        <f t="shared" si="8"/>
+        <v>118.73156509818386</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1709,14 +1844,18 @@
       </c>
       <c r="H34" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I34" s="4">
-        <f t="shared" si="7"/>
-        <v>31.378447330720917</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>76.180375287152572</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J34" s="4">
+        <f t="shared" si="8"/>
+        <v>107.55882261787349</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1746,14 +1885,18 @@
       </c>
       <c r="H35" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I35" s="4">
-        <f t="shared" si="7"/>
-        <v>23.419384596444388</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>73.338146559560528</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J35" s="4">
+        <f t="shared" si="8"/>
+        <v>96.757531156004916</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1783,14 +1926,18 @@
       </c>
       <c r="H36" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I36" s="4">
-        <f t="shared" si="7"/>
-        <v>15.689391779956907</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>70.622222570405157</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J36" s="4">
+        <f t="shared" si="8"/>
+        <v>86.311614350362106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1820,17 +1967,21 @@
       </c>
       <c r="H37" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I37" s="4">
-        <f t="shared" si="7"/>
-        <v>8.1797288101242316</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>68.026103302440063</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J37" s="4">
+        <f t="shared" si="8"/>
+        <v>76.205832112564281</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Co the la nghiem</v>
+        <v>-</v>
       </c>
       <c r="B38" s="3">
         <v>0.35</v>
@@ -1857,14 +2008,18 @@
       </c>
       <c r="H38" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I38" s="4">
-        <f t="shared" si="7"/>
-        <v>0.8820621668255626</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65.54366823898151</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J38" s="4">
+        <f t="shared" si="8"/>
+        <v>66.425730405807087</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1894,14 +2049,18 @@
       </c>
       <c r="H39" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I39" s="4">
-        <f t="shared" si="7"/>
-        <v>-6.2115571981895528</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63.169151618349609</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" si="8"/>
+        <v>56.957594420160035</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1931,14 +2090,18 @@
       </c>
       <c r="H40" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I40" s="4">
-        <f t="shared" si="7"/>
-        <v>-13.108714577401372</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60.897119468214918</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J40" s="4">
+        <f t="shared" si="8"/>
+        <v>47.788404890813524</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1968,14 +2131,18 @@
       </c>
       <c r="H41" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I41" s="4">
-        <f t="shared" si="7"/>
-        <v>-19.816650954481531</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>58.722448280031266</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J41" s="4">
+        <f t="shared" si="8"/>
+        <v>38.905797325549713</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2005,14 +2172,18 @@
       </c>
       <c r="H42" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I42" s="4">
-        <f t="shared" si="7"/>
-        <v>-26.342281268912984</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>56.640305195629821</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J42" s="4">
+        <f t="shared" si="8"/>
+        <v>30.298023926716837</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2042,14 +2213,18 @@
       </c>
       <c r="H43" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I43" s="4">
-        <f t="shared" si="7"/>
-        <v>-32.692211578508932</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>54.646129588861797</v>
+      </c>
+      <c r="I43" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J43" s="4">
+        <f t="shared" si="8"/>
+        <v>21.953918010352879</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2079,17 +2254,21 @@
       </c>
       <c r="H44" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I44" s="4">
-        <f t="shared" si="7"/>
-        <v>-38.872755194093941</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>52.735615934997533</v>
+      </c>
+      <c r="I44" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J44" s="4">
+        <f t="shared" si="8"/>
+        <v>13.862860740903614</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>Co the la nghiem</v>
       </c>
       <c r="B45" s="3">
         <v>0.42</v>
@@ -2116,14 +2295,18 @@
       </c>
       <c r="H45" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I45" s="4">
-        <f t="shared" si="7"/>
-        <v>-44.889947855082823</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50.904697869533777</v>
+      </c>
+      <c r="I45" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J45" s="4">
+        <f t="shared" si="8"/>
+        <v>6.0147500144509536</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2153,14 +2336,18 @@
       </c>
       <c r="H46" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I46" s="4">
-        <f t="shared" si="7"/>
-        <v>-50.749562009640272</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49.149533346194445</v>
+      </c>
+      <c r="I46" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" si="8"/>
+        <v>-1.6000286634458121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2190,14 +2377,18 @@
       </c>
       <c r="H47" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I47" s="4">
-        <f t="shared" si="7"/>
-        <v>-56.45712025844</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>47.466490811325663</v>
+      </c>
+      <c r="I47" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J47" s="4">
+        <f t="shared" si="8"/>
+        <v>-8.9906294471143156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2227,14 +2418,18 @@
       </c>
       <c r="H48" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I48" s="4">
-        <f t="shared" si="7"/>
-        <v>-62.017908016757133</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45.852136318643097</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J48" s="4">
+        <f t="shared" si="8"/>
+        <v>-16.165771698114042</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2264,14 +2459,18 @@
       </c>
       <c r="H49" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I49" s="4">
-        <f t="shared" si="7"/>
-        <v>-67.436985445683035</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44.303221514453519</v>
+      </c>
+      <c r="I49" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J49" s="4">
+        <f t="shared" si="8"/>
+        <v>-23.13376393122951</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2301,14 +2500,18 @@
       </c>
       <c r="H50" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I50" s="4">
-        <f t="shared" si="7"/>
-        <v>-72.719198699610956</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42.816672429099505</v>
+      </c>
+      <c r="I50" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J50" s="4">
+        <f t="shared" si="8"/>
+        <v>-29.90252627051143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2338,14 +2541,18 @@
       </c>
       <c r="H51" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I51" s="4">
-        <f t="shared" si="7"/>
-        <v>-77.869190533790857</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>41.389579015515366</v>
+      </c>
+      <c r="I51" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J51" s="4">
+        <f t="shared" si="8"/>
+        <v>-36.479611518275476</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2375,14 +2582,18 @@
       </c>
       <c r="H52" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I52" s="4">
-        <f t="shared" si="7"/>
-        <v>-82.891410312658707</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>40.019185380478497</v>
+      </c>
+      <c r="I52" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J52" s="4">
+        <f t="shared" si="8"/>
+        <v>-42.872224932180188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2412,14 +2623,18 @@
       </c>
       <c r="H53" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I53" s="4">
-        <f t="shared" si="7"/>
-        <v>-87.790123456790127</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38.702880658436214</v>
+      </c>
+      <c r="I53" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J53" s="4">
+        <f t="shared" si="8"/>
+        <v>-49.087242798353941</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2449,14 +2664,18 @@
       </c>
       <c r="H54" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I54" s="4">
-        <f t="shared" si="7"/>
-        <v>-92.5694203636927</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37.438190481717911</v>
+      </c>
+      <c r="I54" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J54" s="4">
+        <f t="shared" si="8"/>
+        <v>-55.131229881974775</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2486,14 +2705,18 @@
       </c>
       <c r="H55" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I55" s="4">
-        <f t="shared" si="7"/>
-        <v>-97.233224835214628</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36.222769004541007</v>
+      </c>
+      <c r="I55" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J55" s="4">
+        <f t="shared" si="8"/>
+        <v>-61.010455830673607</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2523,14 +2746,18 @@
       </c>
       <c r="H56" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I56" s="4">
-        <f t="shared" si="7"/>
-        <v>-101.78530204209653</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35.054391441516017</v>
+      </c>
+      <c r="I56" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J56" s="4">
+        <f t="shared" si="8"/>
+        <v>-66.730910600580501</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2560,14 +2787,18 @@
       </c>
       <c r="H57" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I57" s="4">
-        <f t="shared" si="7"/>
-        <v>-106.22926605410896</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33.930947084378111</v>
+      </c>
+      <c r="I57" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J57" s="4">
+        <f t="shared" si="8"/>
+        <v>-72.298318969730872</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2597,14 +2828,18 @@
       </c>
       <c r="H58" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I58" s="4">
-        <f t="shared" si="7"/>
-        <v>-110.56858696228892</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32.850432763444495</v>
+      </c>
+      <c r="I58" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J58" s="4">
+        <f t="shared" si="8"/>
+        <v>-77.718154198844445</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2634,14 +2869,18 @@
       </c>
       <c r="H59" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I59" s="4">
-        <f t="shared" si="7"/>
-        <v>-114.80659761800717</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31.810946722840946</v>
+      </c>
+      <c r="I59" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J59" s="4">
+        <f t="shared" si="8"/>
+        <v>-82.99565089516625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2671,14 +2910,18 @@
       </c>
       <c r="H60" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I60" s="4">
-        <f t="shared" si="7"/>
-        <v>-118.94650001193844</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30.810682880876342</v>
+      </c>
+      <c r="I60" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J60" s="4">
+        <f t="shared" si="8"/>
+        <v>-88.135817131062083</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2708,14 +2951,18 @@
       </c>
       <c r="H61" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I61" s="4">
-        <f t="shared" si="7"/>
-        <v>-122.99137131447822</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29.847925449090855</v>
+      </c>
+      <c r="I61" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J61" s="4">
+        <f t="shared" si="8"/>
+        <v>-93.143445865387378</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2745,14 +2992,18 @@
       </c>
       <c r="H62" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I62" s="4">
-        <f t="shared" si="7"/>
-        <v>-126.94416959772218</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28.921043885476124</v>
+      </c>
+      <c r="I62" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J62" s="4">
+        <f t="shared" si="8"/>
+        <v>-98.023125712246042</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2782,14 +3033,18 @@
       </c>
       <c r="H63" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I63" s="4">
-        <f t="shared" si="7"/>
-        <v>-130.8077392578125</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28.02848815917967</v>
+      </c>
+      <c r="I63" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J63" s="4">
+        <f t="shared" si="8"/>
+        <v>-102.77925109863281</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2819,14 +3074,18 @@
       </c>
       <c r="H64" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I64" s="4">
-        <f t="shared" si="7"/>
-        <v>-134.5848161552189</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27.168784305677587</v>
+      </c>
+      <c r="I64" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J64" s="4">
+        <f t="shared" si="8"/>
+        <v>-107.4160318495413</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2856,14 +3115,18 @@
       </c>
       <c r="H65" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I65" s="4">
-        <f t="shared" si="7"/>
-        <v>-138.27803248939688</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26.340530252934315</v>
+      </c>
+      <c r="I65" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J65" s="4">
+        <f t="shared" si="8"/>
+        <v>-111.93750223646259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2893,14 +3156,18 @@
       </c>
       <c r="H66" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I66" s="4">
-        <f t="shared" si="7"/>
-        <v>-141.88992142319609</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25.542391900488212</v>
+      </c>
+      <c r="I66" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J66" s="4">
+        <f t="shared" si="8"/>
+        <v>-116.34752952270787</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2930,1343 +3197,1491 @@
       </c>
       <c r="H67" s="3">
         <f t="shared" si="6"/>
-        <v>-430</v>
-      </c>
-      <c r="I67" s="4">
-        <f t="shared" si="7"/>
-        <v>-145.42292147141956</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24.773099434703532</v>
+      </c>
+      <c r="I67" s="3">
+        <f t="shared" si="7"/>
+        <v>-430</v>
+      </c>
+      <c r="J67" s="4">
+        <f t="shared" si="8"/>
+        <v>-120.64982203671605</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="str">
-        <f t="shared" ref="A68:A103" si="8">IF(AND(0&lt;I68,I68*I69&lt;0),"Co the la nghiem","-")</f>
+        <f t="shared" ref="A68:A103" si="9">IF(AND(0&lt;J68,J68*J69&lt;0),"Co the la nghiem","-")</f>
         <v>-</v>
       </c>
       <c r="B68" s="3">
         <v>0.65</v>
       </c>
       <c r="C68" s="3">
-        <f t="shared" ref="C68:C103" si="9">1+B68</f>
+        <f t="shared" ref="C68:C103" si="10">1+B68</f>
         <v>1.65</v>
       </c>
       <c r="D68" s="3">
-        <f t="shared" ref="D68:D103" si="10">$D$1/C68</f>
+        <f t="shared" ref="D68:D103" si="11">$D$1/C68</f>
         <v>122.36363636363637</v>
       </c>
       <c r="E68" s="3">
-        <f t="shared" ref="E68:E103" si="11">$E$1/(C68^2)</f>
+        <f t="shared" ref="E68:E103" si="12">$E$1/(C68^2)</f>
         <v>74.159779614325075</v>
       </c>
       <c r="F68" s="3">
-        <f t="shared" ref="F68:F103" si="12">$F$1/(C68^3)</f>
+        <f t="shared" ref="F68:F103" si="13">$F$1/(C68^3)</f>
         <v>44.945320978378831</v>
       </c>
       <c r="G68" s="3">
-        <f t="shared" ref="G68:G103" si="13">$G$1/(C68^4)</f>
+        <f t="shared" ref="G68:G103" si="14">$G$1/(C68^4)</f>
         <v>39.651882376650725</v>
       </c>
       <c r="H68" s="3">
-        <f t="shared" ref="H68:H103" si="14">$H$1</f>
-        <v>-430</v>
-      </c>
-      <c r="I68" s="4">
-        <f t="shared" ref="I68:I103" si="15">SUM(D68:H68)</f>
-        <v>-148.87938066700895</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H68:H103" si="15">$H$1/(C68^5)</f>
+        <v>24.031443864636806</v>
+      </c>
+      <c r="I68" s="3">
+        <f t="shared" ref="I68:I103" si="16">$I$1</f>
+        <v>-430</v>
+      </c>
+      <c r="J68" s="4">
+        <f t="shared" ref="J68:J103" si="17">SUM(D68:I68)</f>
+        <v>-124.84793680237215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-</v>
       </c>
       <c r="B69" s="3">
         <v>0.66</v>
       </c>
       <c r="C69" s="3">
+        <f t="shared" si="10"/>
+        <v>1.6600000000000001</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="11"/>
+        <v>121.62650602409637</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="12"/>
+        <v>73.268979532588176</v>
+      </c>
+      <c r="F69" s="3">
+        <f t="shared" si="13"/>
+        <v>44.137939477462751</v>
+      </c>
+      <c r="G69" s="3">
+        <f t="shared" si="14"/>
+        <v>38.70501444836195</v>
+      </c>
+      <c r="H69" s="3">
+        <f t="shared" si="15"/>
+        <v>23.316273764073461</v>
+      </c>
+      <c r="I69" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J69" s="4">
+        <f t="shared" si="17"/>
+        <v>-128.94528675341729</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.6600000000000001</v>
-      </c>
-      <c r="D69" s="3">
-        <f t="shared" si="10"/>
-        <v>121.62650602409637</v>
-      </c>
-      <c r="E69" s="3">
-        <f t="shared" si="11"/>
-        <v>73.268979532588176</v>
-      </c>
-      <c r="F69" s="3">
-        <f t="shared" si="12"/>
-        <v>44.137939477462751</v>
-      </c>
-      <c r="G69" s="3">
-        <f t="shared" si="13"/>
-        <v>38.70501444836195</v>
-      </c>
-      <c r="H69" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I69" s="4">
-        <f t="shared" si="15"/>
-        <v>-152.26156051749075</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B70" s="3">
         <v>0.67</v>
       </c>
       <c r="C70" s="3">
+        <f t="shared" si="10"/>
+        <v>1.67</v>
+      </c>
+      <c r="D70" s="3">
+        <f t="shared" si="11"/>
+        <v>120.89820359281438</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="12"/>
+        <v>72.394133887912801</v>
+      </c>
+      <c r="F70" s="3">
+        <f t="shared" si="13"/>
+        <v>43.349780771205268</v>
+      </c>
+      <c r="G70" s="3">
+        <f t="shared" si="14"/>
+        <v>37.786241984551637</v>
+      </c>
+      <c r="H70" s="3">
+        <f t="shared" si="15"/>
+        <v>22.626492206318346</v>
+      </c>
+      <c r="I70" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J70" s="4">
+        <f t="shared" si="17"/>
+        <v>-132.94514755719757</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.67</v>
-      </c>
-      <c r="D70" s="3">
-        <f t="shared" si="10"/>
-        <v>120.89820359281438</v>
-      </c>
-      <c r="E70" s="3">
-        <f t="shared" si="11"/>
-        <v>72.394133887912801</v>
-      </c>
-      <c r="F70" s="3">
-        <f t="shared" si="12"/>
-        <v>43.349780771205268</v>
-      </c>
-      <c r="G70" s="3">
-        <f t="shared" si="13"/>
-        <v>37.786241984551637</v>
-      </c>
-      <c r="H70" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I70" s="4">
-        <f t="shared" si="15"/>
-        <v>-155.57163976351592</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B71" s="3">
         <v>0.68</v>
       </c>
       <c r="C71" s="3">
+        <f t="shared" si="10"/>
+        <v>1.6800000000000002</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="11"/>
+        <v>120.17857142857142</v>
+      </c>
+      <c r="E71" s="3">
+        <f t="shared" si="12"/>
+        <v>71.534863945578223</v>
+      </c>
+      <c r="F71" s="3">
+        <f t="shared" si="13"/>
+        <v>42.58027615808227</v>
+      </c>
+      <c r="G71" s="3">
+        <f t="shared" si="14"/>
+        <v>36.894570517171331</v>
+      </c>
+      <c r="H71" s="3">
+        <f t="shared" si="15"/>
+        <v>21.961053879268647</v>
+      </c>
+      <c r="I71" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J71" s="4">
+        <f t="shared" si="17"/>
+        <v>-136.85066407132808</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.6800000000000002</v>
-      </c>
-      <c r="D71" s="3">
-        <f t="shared" si="10"/>
-        <v>120.17857142857142</v>
-      </c>
-      <c r="E71" s="3">
-        <f t="shared" si="11"/>
-        <v>71.534863945578223</v>
-      </c>
-      <c r="F71" s="3">
-        <f t="shared" si="12"/>
-        <v>42.58027615808227</v>
-      </c>
-      <c r="G71" s="3">
-        <f t="shared" si="13"/>
-        <v>36.894570517171331</v>
-      </c>
-      <c r="H71" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I71" s="4">
-        <f t="shared" si="15"/>
-        <v>-158.81171795059674</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B72" s="3">
         <v>0.69</v>
       </c>
       <c r="C72" s="3">
+        <f t="shared" si="10"/>
+        <v>1.69</v>
+      </c>
+      <c r="D72" s="3">
+        <f t="shared" si="11"/>
+        <v>119.46745562130178</v>
+      </c>
+      <c r="E72" s="3">
+        <f t="shared" si="12"/>
+        <v>70.690802142782132</v>
+      </c>
+      <c r="F72" s="3">
+        <f t="shared" si="13"/>
+        <v>41.828877007563392</v>
+      </c>
+      <c r="G72" s="3">
+        <f t="shared" si="14"/>
+        <v>36.029046403905156</v>
+      </c>
+      <c r="H72" s="3">
+        <f t="shared" si="15"/>
+        <v>21.318962369174649</v>
+      </c>
+      <c r="I72" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J72" s="4">
+        <f t="shared" si="17"/>
+        <v>-140.66485645527291</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.69</v>
-      </c>
-      <c r="D72" s="3">
-        <f t="shared" si="10"/>
-        <v>119.46745562130178</v>
-      </c>
-      <c r="E72" s="3">
-        <f t="shared" si="11"/>
-        <v>70.690802142782132</v>
-      </c>
-      <c r="F72" s="3">
-        <f t="shared" si="12"/>
-        <v>41.828877007563392</v>
-      </c>
-      <c r="G72" s="3">
-        <f t="shared" si="13"/>
-        <v>36.029046403905156</v>
-      </c>
-      <c r="H72" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I72" s="4">
-        <f t="shared" si="15"/>
-        <v>-161.98381882444755</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B73" s="3">
         <v>0.7</v>
       </c>
       <c r="C73" s="3">
+        <f t="shared" si="10"/>
+        <v>1.7</v>
+      </c>
+      <c r="D73" s="3">
+        <f t="shared" si="11"/>
+        <v>118.76470588235294</v>
+      </c>
+      <c r="E73" s="3">
+        <f t="shared" si="12"/>
+        <v>69.861591695501744</v>
+      </c>
+      <c r="F73" s="3">
+        <f t="shared" si="13"/>
+        <v>41.095053938530434</v>
+      </c>
+      <c r="G73" s="3">
+        <f t="shared" si="14"/>
+        <v>35.188754923911354</v>
+      </c>
+      <c r="H73" s="3">
+        <f t="shared" si="15"/>
+        <v>20.6992676023008</v>
+      </c>
+      <c r="I73" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J73" s="4">
+        <f t="shared" si="17"/>
+        <v>-144.39062595740273</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.7</v>
-      </c>
-      <c r="D73" s="3">
-        <f t="shared" si="10"/>
-        <v>118.76470588235294</v>
-      </c>
-      <c r="E73" s="3">
-        <f t="shared" si="11"/>
-        <v>69.861591695501744</v>
-      </c>
-      <c r="F73" s="3">
-        <f t="shared" si="12"/>
-        <v>41.095053938530434</v>
-      </c>
-      <c r="G73" s="3">
-        <f t="shared" si="13"/>
-        <v>35.188754923911354</v>
-      </c>
-      <c r="H73" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I73" s="4">
-        <f t="shared" si="15"/>
-        <v>-165.08989355970351</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B74" s="3">
         <v>0.71</v>
       </c>
       <c r="C74" s="3">
+        <f t="shared" si="10"/>
+        <v>1.71</v>
+      </c>
+      <c r="D74" s="3">
+        <f t="shared" si="11"/>
+        <v>118.07017543859649</v>
+      </c>
+      <c r="E74" s="3">
+        <f t="shared" si="12"/>
+        <v>69.046886221401465</v>
+      </c>
+      <c r="F74" s="3">
+        <f t="shared" si="13"/>
+        <v>40.37829603590729</v>
+      </c>
+      <c r="G74" s="3">
+        <f t="shared" si="14"/>
+        <v>34.372818472908399</v>
+      </c>
+      <c r="H74" s="3">
+        <f t="shared" si="15"/>
+        <v>20.101063434449355</v>
+      </c>
+      <c r="I74" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J74" s="4">
+        <f t="shared" si="17"/>
+        <v>-148.03076039673698</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.71</v>
-      </c>
-      <c r="D74" s="3">
-        <f t="shared" si="10"/>
-        <v>118.07017543859649</v>
-      </c>
-      <c r="E74" s="3">
-        <f t="shared" si="11"/>
-        <v>69.046886221401465</v>
-      </c>
-      <c r="F74" s="3">
-        <f t="shared" si="12"/>
-        <v>40.37829603590729</v>
-      </c>
-      <c r="G74" s="3">
-        <f t="shared" si="13"/>
-        <v>34.372818472908399</v>
-      </c>
-      <c r="H74" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I74" s="4">
-        <f t="shared" si="15"/>
-        <v>-168.13182383118635</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B75" s="3">
         <v>0.72</v>
       </c>
       <c r="C75" s="3">
+        <f t="shared" si="10"/>
+        <v>1.72</v>
+      </c>
+      <c r="D75" s="3">
+        <f t="shared" si="11"/>
+        <v>117.38372093023256</v>
+      </c>
+      <c r="E75" s="3">
+        <f t="shared" si="12"/>
+        <v>68.246349378042197</v>
+      </c>
+      <c r="F75" s="3">
+        <f t="shared" si="13"/>
+        <v>39.6781101035129</v>
+      </c>
+      <c r="G75" s="3">
+        <f t="shared" si="14"/>
+        <v>33.580394851879362</v>
+      </c>
+      <c r="H75" s="3">
+        <f t="shared" si="15"/>
+        <v>19.523485378999631</v>
+      </c>
+      <c r="I75" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J75" s="4">
+        <f t="shared" si="17"/>
+        <v>-151.58793935733337</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.72</v>
-      </c>
-      <c r="D75" s="3">
-        <f t="shared" si="10"/>
-        <v>117.38372093023256</v>
-      </c>
-      <c r="E75" s="3">
-        <f t="shared" si="11"/>
-        <v>68.246349378042197</v>
-      </c>
-      <c r="F75" s="3">
-        <f t="shared" si="12"/>
-        <v>39.6781101035129</v>
-      </c>
-      <c r="G75" s="3">
-        <f t="shared" si="13"/>
-        <v>33.580394851879362</v>
-      </c>
-      <c r="H75" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I75" s="4">
-        <f t="shared" si="15"/>
-        <v>-171.11142473633299</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B76" s="3">
         <v>0.73</v>
       </c>
       <c r="C76" s="3">
+        <f t="shared" si="10"/>
+        <v>1.73</v>
+      </c>
+      <c r="D76" s="3">
+        <f t="shared" si="11"/>
+        <v>116.70520231213874</v>
+      </c>
+      <c r="E76" s="3">
+        <f t="shared" si="12"/>
+        <v>67.45965451568712</v>
+      </c>
+      <c r="F76" s="3">
+        <f t="shared" si="13"/>
+        <v>38.994019951264235</v>
+      </c>
+      <c r="G76" s="3">
+        <f t="shared" si="14"/>
+        <v>32.810675644030717</v>
+      </c>
+      <c r="H76" s="3">
+        <f t="shared" si="15"/>
+        <v>18.96570846475764</v>
+      </c>
+      <c r="I76" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J76" s="4">
+        <f t="shared" si="17"/>
+        <v>-155.06473911212152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.73</v>
-      </c>
-      <c r="D76" s="3">
-        <f t="shared" si="10"/>
-        <v>116.70520231213874</v>
-      </c>
-      <c r="E76" s="3">
-        <f t="shared" si="11"/>
-        <v>67.45965451568712</v>
-      </c>
-      <c r="F76" s="3">
-        <f t="shared" si="12"/>
-        <v>38.994019951264235</v>
-      </c>
-      <c r="G76" s="3">
-        <f t="shared" si="13"/>
-        <v>32.810675644030717</v>
-      </c>
-      <c r="H76" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I76" s="4">
-        <f t="shared" si="15"/>
-        <v>-174.03044757687917</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B77" s="3">
         <v>0.74</v>
       </c>
       <c r="C77" s="3">
+        <f t="shared" si="10"/>
+        <v>1.74</v>
+      </c>
+      <c r="D77" s="3">
+        <f t="shared" si="11"/>
+        <v>116.0344827586207</v>
+      </c>
+      <c r="E77" s="3">
+        <f t="shared" si="12"/>
+        <v>66.686484344034881</v>
+      </c>
+      <c r="F77" s="3">
+        <f t="shared" si="13"/>
+        <v>38.325565714962572</v>
+      </c>
+      <c r="G77" s="3">
+        <f t="shared" si="14"/>
+        <v>32.062884674977084</v>
+      </c>
+      <c r="H77" s="3">
+        <f t="shared" si="15"/>
+        <v>18.42694521550407</v>
+      </c>
+      <c r="I77" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J77" s="4">
+        <f t="shared" si="17"/>
+        <v>-158.46363729190068</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.74</v>
-      </c>
-      <c r="D77" s="3">
-        <f t="shared" si="10"/>
-        <v>116.0344827586207</v>
-      </c>
-      <c r="E77" s="3">
-        <f t="shared" si="11"/>
-        <v>66.686484344034881</v>
-      </c>
-      <c r="F77" s="3">
-        <f t="shared" si="12"/>
-        <v>38.325565714962572</v>
-      </c>
-      <c r="G77" s="3">
-        <f t="shared" si="13"/>
-        <v>32.062884674977084</v>
-      </c>
-      <c r="H77" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I77" s="4">
-        <f t="shared" si="15"/>
-        <v>-176.89058250740476</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B78" s="3">
         <v>0.75</v>
       </c>
       <c r="C78" s="3">
+        <f t="shared" si="10"/>
+        <v>1.75</v>
+      </c>
+      <c r="D78" s="3">
+        <f t="shared" si="11"/>
+        <v>115.37142857142858</v>
+      </c>
+      <c r="E78" s="3">
+        <f t="shared" si="12"/>
+        <v>65.926530612244903</v>
+      </c>
+      <c r="F78" s="3">
+        <f t="shared" si="13"/>
+        <v>37.672303206997086</v>
+      </c>
+      <c r="G78" s="3">
+        <f t="shared" si="14"/>
+        <v>31.336276551436899</v>
+      </c>
+      <c r="H78" s="3">
+        <f t="shared" si="15"/>
+        <v>17.906443743678228</v>
+      </c>
+      <c r="I78" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J78" s="4">
+        <f t="shared" si="17"/>
+        <v>-161.78701731421432</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.75</v>
-      </c>
-      <c r="D78" s="3">
-        <f t="shared" si="10"/>
-        <v>115.37142857142858</v>
-      </c>
-      <c r="E78" s="3">
-        <f t="shared" si="11"/>
-        <v>65.926530612244903</v>
-      </c>
-      <c r="F78" s="3">
-        <f t="shared" si="12"/>
-        <v>37.672303206997086</v>
-      </c>
-      <c r="G78" s="3">
-        <f t="shared" si="13"/>
-        <v>31.336276551436899</v>
-      </c>
-      <c r="H78" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I78" s="4">
-        <f t="shared" si="15"/>
-        <v>-179.69346105789256</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B79" s="3">
         <v>0.76</v>
       </c>
       <c r="C79" s="3">
+        <f t="shared" si="10"/>
+        <v>1.76</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="11"/>
+        <v>114.71590909090909</v>
+      </c>
+      <c r="E79" s="3">
+        <f t="shared" si="12"/>
+        <v>65.179493801652896</v>
+      </c>
+      <c r="F79" s="3">
+        <f t="shared" si="13"/>
+        <v>37.033803296393693</v>
+      </c>
+      <c r="G79" s="3">
+        <f t="shared" si="14"/>
+        <v>30.630135274016457</v>
+      </c>
+      <c r="H79" s="3">
+        <f t="shared" si="15"/>
+        <v>17.403485951145715</v>
+      </c>
+      <c r="I79" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J79" s="4">
+        <f t="shared" si="17"/>
+        <v>-165.0371725858821</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.76</v>
-      </c>
-      <c r="D79" s="3">
-        <f t="shared" si="10"/>
-        <v>114.71590909090909</v>
-      </c>
-      <c r="E79" s="3">
-        <f t="shared" si="11"/>
-        <v>65.179493801652896</v>
-      </c>
-      <c r="F79" s="3">
-        <f t="shared" si="12"/>
-        <v>37.033803296393693</v>
-      </c>
-      <c r="G79" s="3">
-        <f t="shared" si="13"/>
-        <v>30.630135274016457</v>
-      </c>
-      <c r="H79" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I79" s="4">
-        <f t="shared" si="15"/>
-        <v>-182.44065853702784</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B80" s="3">
         <v>0.77</v>
       </c>
       <c r="C80" s="3">
+        <f t="shared" si="10"/>
+        <v>1.77</v>
+      </c>
+      <c r="D80" s="3">
+        <f t="shared" si="11"/>
+        <v>114.06779661016949</v>
+      </c>
+      <c r="E80" s="3">
+        <f t="shared" si="12"/>
+        <v>64.445082830604235</v>
+      </c>
+      <c r="F80" s="3">
+        <f t="shared" si="13"/>
+        <v>36.409651316725551</v>
+      </c>
+      <c r="G80" s="3">
+        <f t="shared" si="14"/>
+        <v>29.943772919931941</v>
+      </c>
+      <c r="H80" s="3">
+        <f t="shared" si="15"/>
+        <v>16.917385830470025</v>
+      </c>
+      <c r="I80" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J80" s="4">
+        <f t="shared" si="17"/>
+        <v>-168.21631049209873</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.77</v>
-      </c>
-      <c r="D80" s="3">
-        <f t="shared" si="10"/>
-        <v>114.06779661016949</v>
-      </c>
-      <c r="E80" s="3">
-        <f t="shared" si="11"/>
-        <v>64.445082830604235</v>
-      </c>
-      <c r="F80" s="3">
-        <f t="shared" si="12"/>
-        <v>36.409651316725551</v>
-      </c>
-      <c r="G80" s="3">
-        <f t="shared" si="13"/>
-        <v>29.943772919931941</v>
-      </c>
-      <c r="H80" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I80" s="4">
-        <f t="shared" si="15"/>
-        <v>-185.13369632256877</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B81" s="3">
         <v>0.78</v>
       </c>
       <c r="C81" s="3">
+        <f t="shared" si="10"/>
+        <v>1.78</v>
+      </c>
+      <c r="D81" s="3">
+        <f t="shared" si="11"/>
+        <v>113.42696629213484</v>
+      </c>
+      <c r="E81" s="3">
+        <f t="shared" si="12"/>
+        <v>63.723014770862264</v>
+      </c>
+      <c r="F81" s="3">
+        <f t="shared" si="13"/>
+        <v>35.799446500484414</v>
+      </c>
+      <c r="G81" s="3">
+        <f t="shared" si="14"/>
+        <v>29.276528391773567</v>
+      </c>
+      <c r="H81" s="3">
+        <f t="shared" si="15"/>
+        <v>16.44748786054695</v>
+      </c>
+      <c r="I81" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J81" s="4">
+        <f t="shared" si="17"/>
+        <v>-171.32655618419795</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.78</v>
-      </c>
-      <c r="D81" s="3">
-        <f t="shared" si="10"/>
-        <v>113.42696629213484</v>
-      </c>
-      <c r="E81" s="3">
-        <f t="shared" si="11"/>
-        <v>63.723014770862264</v>
-      </c>
-      <c r="F81" s="3">
-        <f t="shared" si="12"/>
-        <v>35.799446500484414</v>
-      </c>
-      <c r="G81" s="3">
-        <f t="shared" si="13"/>
-        <v>29.276528391773567</v>
-      </c>
-      <c r="H81" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I81" s="4">
-        <f t="shared" si="15"/>
-        <v>-187.77404404474493</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B82" s="3">
         <v>0.79</v>
       </c>
       <c r="C82" s="3">
+        <f t="shared" si="10"/>
+        <v>1.79</v>
+      </c>
+      <c r="D82" s="3">
+        <f t="shared" si="11"/>
+        <v>112.79329608938548</v>
+      </c>
+      <c r="E82" s="3">
+        <f t="shared" si="12"/>
+        <v>63.013014575075687</v>
+      </c>
+      <c r="F82" s="3">
+        <f t="shared" si="13"/>
+        <v>35.202801438589773</v>
+      </c>
+      <c r="G82" s="3">
+        <f t="shared" si="14"/>
+        <v>28.627766228653304</v>
+      </c>
+      <c r="H82" s="3">
+        <f t="shared" si="15"/>
+        <v>15.993165490867765</v>
+      </c>
+      <c r="I82" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J82" s="4">
+        <f t="shared" si="17"/>
+        <v>-174.36995617742798</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.79</v>
-      </c>
-      <c r="D82" s="3">
-        <f t="shared" si="10"/>
-        <v>112.79329608938548</v>
-      </c>
-      <c r="E82" s="3">
-        <f t="shared" si="11"/>
-        <v>63.013014575075687</v>
-      </c>
-      <c r="F82" s="3">
-        <f t="shared" si="12"/>
-        <v>35.202801438589773</v>
-      </c>
-      <c r="G82" s="3">
-        <f t="shared" si="13"/>
-        <v>28.627766228653304</v>
-      </c>
-      <c r="H82" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I82" s="4">
-        <f t="shared" si="15"/>
-        <v>-190.36312166829575</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B83" s="3">
         <v>0.8</v>
       </c>
       <c r="C83" s="3">
+        <f t="shared" si="10"/>
+        <v>1.8</v>
+      </c>
+      <c r="D83" s="3">
+        <f t="shared" si="11"/>
+        <v>112.16666666666667</v>
+      </c>
+      <c r="E83" s="3">
+        <f t="shared" si="12"/>
+        <v>62.31481481481481</v>
+      </c>
+      <c r="F83" s="3">
+        <f t="shared" si="13"/>
+        <v>34.619341563786001</v>
+      </c>
+      <c r="G83" s="3">
+        <f t="shared" si="14"/>
+        <v>27.996875476299337</v>
+      </c>
+      <c r="H83" s="3">
+        <f t="shared" si="15"/>
+        <v>15.553819709055185</v>
+      </c>
+      <c r="I83" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J83" s="4">
+        <f t="shared" si="17"/>
+        <v>-177.348481769378</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.8</v>
-      </c>
-      <c r="D83" s="3">
-        <f t="shared" si="10"/>
-        <v>112.16666666666667</v>
-      </c>
-      <c r="E83" s="3">
-        <f t="shared" si="11"/>
-        <v>62.31481481481481</v>
-      </c>
-      <c r="F83" s="3">
-        <f t="shared" si="12"/>
-        <v>34.619341563786001</v>
-      </c>
-      <c r="G83" s="3">
-        <f t="shared" si="13"/>
-        <v>27.996875476299337</v>
-      </c>
-      <c r="H83" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I83" s="4">
-        <f t="shared" si="15"/>
-        <v>-192.90230147843317</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B84" s="3">
         <v>0.81</v>
       </c>
       <c r="C84" s="3">
+        <f t="shared" si="10"/>
+        <v>1.81</v>
+      </c>
+      <c r="D84" s="3">
+        <f t="shared" si="11"/>
+        <v>111.54696132596685</v>
+      </c>
+      <c r="E84" s="3">
+        <f t="shared" si="12"/>
+        <v>61.628155428710969</v>
+      </c>
+      <c r="F84" s="3">
+        <f t="shared" si="13"/>
+        <v>34.048704656746395</v>
+      </c>
+      <c r="G84" s="3">
+        <f t="shared" si="14"/>
+        <v>27.38326861286771</v>
+      </c>
+      <c r="H84" s="3">
+        <f t="shared" si="15"/>
+        <v>15.128877686667243</v>
+      </c>
+      <c r="I84" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J84" s="4">
+        <f t="shared" si="17"/>
+        <v>-180.26403228904084</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.81</v>
-      </c>
-      <c r="D84" s="3">
-        <f t="shared" si="10"/>
-        <v>111.54696132596685</v>
-      </c>
-      <c r="E84" s="3">
-        <f t="shared" si="11"/>
-        <v>61.628155428710969</v>
-      </c>
-      <c r="F84" s="3">
-        <f t="shared" si="12"/>
-        <v>34.048704656746395</v>
-      </c>
-      <c r="G84" s="3">
-        <f t="shared" si="13"/>
-        <v>27.38326861286771</v>
-      </c>
-      <c r="H84" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I84" s="4">
-        <f t="shared" si="15"/>
-        <v>-195.39290997570808</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B85" s="3">
         <v>0.82</v>
       </c>
       <c r="C85" s="3">
+        <f t="shared" si="10"/>
+        <v>1.8199999999999998</v>
+      </c>
+      <c r="D85" s="3">
+        <f t="shared" si="11"/>
+        <v>110.93406593406594</v>
+      </c>
+      <c r="E85" s="3">
+        <f t="shared" si="12"/>
+        <v>60.952783480256024</v>
+      </c>
+      <c r="F85" s="3">
+        <f t="shared" si="13"/>
+        <v>33.490540373767047</v>
+      </c>
+      <c r="G85" s="3">
+        <f t="shared" si="14"/>
+        <v>26.786380527434797</v>
+      </c>
+      <c r="H85" s="3">
+        <f t="shared" si="15"/>
+        <v>14.71779149859055</v>
+      </c>
+      <c r="I85" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J85" s="4">
+        <f t="shared" si="17"/>
+        <v>-183.11843818588562</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.8199999999999998</v>
-      </c>
-      <c r="D85" s="3">
-        <f t="shared" si="10"/>
-        <v>110.93406593406594</v>
-      </c>
-      <c r="E85" s="3">
-        <f t="shared" si="11"/>
-        <v>60.952783480256024</v>
-      </c>
-      <c r="F85" s="3">
-        <f t="shared" si="12"/>
-        <v>33.490540373767047</v>
-      </c>
-      <c r="G85" s="3">
-        <f t="shared" si="13"/>
-        <v>26.786380527434797</v>
-      </c>
-      <c r="H85" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I85" s="4">
-        <f t="shared" si="15"/>
-        <v>-197.83622968447617</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B86" s="3">
         <v>0.83</v>
       </c>
       <c r="C86" s="3">
+        <f t="shared" si="10"/>
+        <v>1.83</v>
+      </c>
+      <c r="D86" s="3">
+        <f t="shared" si="11"/>
+        <v>110.32786885245902</v>
+      </c>
+      <c r="E86" s="3">
+        <f t="shared" si="12"/>
+        <v>60.288452924840989</v>
+      </c>
+      <c r="F86" s="3">
+        <f t="shared" si="13"/>
+        <v>32.944509794995078</v>
+      </c>
+      <c r="G86" s="3">
+        <f t="shared" si="14"/>
+        <v>26.205667548315727</v>
+      </c>
+      <c r="H86" s="3">
+        <f t="shared" si="15"/>
+        <v>14.320036911647938</v>
+      </c>
+      <c r="I86" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J86" s="4">
+        <f t="shared" si="17"/>
+        <v>-185.91346396774125</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.83</v>
-      </c>
-      <c r="D86" s="3">
-        <f t="shared" si="10"/>
-        <v>110.32786885245902</v>
-      </c>
-      <c r="E86" s="3">
-        <f t="shared" si="11"/>
-        <v>60.288452924840989</v>
-      </c>
-      <c r="F86" s="3">
-        <f t="shared" si="12"/>
-        <v>32.944509794995078</v>
-      </c>
-      <c r="G86" s="3">
-        <f t="shared" si="13"/>
-        <v>26.205667548315727</v>
-      </c>
-      <c r="H86" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I86" s="4">
-        <f t="shared" si="15"/>
-        <v>-200.2335008793892</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B87" s="3">
         <v>0.84</v>
       </c>
       <c r="C87" s="3">
+        <f t="shared" si="10"/>
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="D87" s="3">
+        <f t="shared" si="11"/>
+        <v>109.72826086956523</v>
+      </c>
+      <c r="E87" s="3">
+        <f t="shared" si="12"/>
+        <v>59.634924385633283</v>
+      </c>
+      <c r="F87" s="3">
+        <f t="shared" si="13"/>
+        <v>32.410284992192004</v>
+      </c>
+      <c r="G87" s="3">
+        <f t="shared" si="14"/>
+        <v>25.640606518523025</v>
+      </c>
+      <c r="H87" s="3">
+        <f t="shared" si="15"/>
+        <v>13.935112238327733</v>
+      </c>
+      <c r="I87" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J87" s="4">
+        <f t="shared" si="17"/>
+        <v>-188.65081099575872</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.8399999999999999</v>
-      </c>
-      <c r="D87" s="3">
-        <f t="shared" si="10"/>
-        <v>109.72826086956523</v>
-      </c>
-      <c r="E87" s="3">
-        <f t="shared" si="11"/>
-        <v>59.634924385633283</v>
-      </c>
-      <c r="F87" s="3">
-        <f t="shared" si="12"/>
-        <v>32.410284992192004</v>
-      </c>
-      <c r="G87" s="3">
-        <f t="shared" si="13"/>
-        <v>25.640606518523025</v>
-      </c>
-      <c r="H87" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I87" s="4">
-        <f t="shared" si="15"/>
-        <v>-202.58592323408647</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B88" s="3">
         <v>0.85</v>
       </c>
       <c r="C88" s="3">
+        <f t="shared" si="10"/>
+        <v>1.85</v>
+      </c>
+      <c r="D88" s="3">
+        <f t="shared" si="11"/>
+        <v>109.13513513513513</v>
+      </c>
+      <c r="E88" s="3">
+        <f t="shared" si="12"/>
+        <v>58.991964937910879</v>
+      </c>
+      <c r="F88" s="3">
+        <f t="shared" si="13"/>
+        <v>31.88754861508696</v>
+      </c>
+      <c r="G88" s="3">
+        <f t="shared" si="14"/>
+        <v>25.090693915837534</v>
+      </c>
+      <c r="H88" s="3">
+        <f t="shared" si="15"/>
+        <v>13.562537251804072</v>
+      </c>
+      <c r="I88" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J88" s="4">
+        <f t="shared" si="17"/>
+        <v>-191.33212014422546</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.85</v>
-      </c>
-      <c r="D88" s="3">
-        <f t="shared" si="10"/>
-        <v>109.13513513513513</v>
-      </c>
-      <c r="E88" s="3">
-        <f t="shared" si="11"/>
-        <v>58.991964937910879</v>
-      </c>
-      <c r="F88" s="3">
-        <f t="shared" si="12"/>
-        <v>31.88754861508696</v>
-      </c>
-      <c r="G88" s="3">
-        <f t="shared" si="13"/>
-        <v>25.090693915837534</v>
-      </c>
-      <c r="H88" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I88" s="4">
-        <f t="shared" si="15"/>
-        <v>-204.89465739602952</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B89" s="3">
         <v>0.86</v>
       </c>
       <c r="C89" s="3">
+        <f t="shared" si="10"/>
+        <v>1.8599999999999999</v>
+      </c>
+      <c r="D89" s="3">
+        <f t="shared" si="11"/>
+        <v>108.54838709677421</v>
+      </c>
+      <c r="E89" s="3">
+        <f t="shared" si="12"/>
+        <v>58.35934790149151</v>
+      </c>
+      <c r="F89" s="3">
+        <f t="shared" si="13"/>
+        <v>31.375993495425544</v>
+      </c>
+      <c r="G89" s="3">
+        <f t="shared" si="14"/>
+        <v>24.555445015113328</v>
+      </c>
+      <c r="H89" s="3">
+        <f t="shared" si="15"/>
+        <v>13.20185215866308</v>
+      </c>
+      <c r="I89" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J89" s="4">
+        <f t="shared" si="17"/>
+        <v>-193.95897433253234</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.8599999999999999</v>
-      </c>
-      <c r="D89" s="3">
-        <f t="shared" si="10"/>
-        <v>108.54838709677421</v>
-      </c>
-      <c r="E89" s="3">
-        <f t="shared" si="11"/>
-        <v>58.35934790149151</v>
-      </c>
-      <c r="F89" s="3">
-        <f t="shared" si="12"/>
-        <v>31.375993495425544</v>
-      </c>
-      <c r="G89" s="3">
-        <f t="shared" si="13"/>
-        <v>24.555445015113328</v>
-      </c>
-      <c r="H89" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I89" s="4">
-        <f t="shared" si="15"/>
-        <v>-207.16082649119542</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B90" s="3">
         <v>0.87</v>
       </c>
       <c r="C90" s="3">
+        <f t="shared" si="10"/>
+        <v>1.87</v>
+      </c>
+      <c r="D90" s="3">
+        <f t="shared" si="11"/>
+        <v>107.96791443850267</v>
+      </c>
+      <c r="E90" s="3">
+        <f t="shared" si="12"/>
+        <v>57.736852640910513</v>
+      </c>
+      <c r="F90" s="3">
+        <f t="shared" si="13"/>
+        <v>30.875322267866583</v>
+      </c>
+      <c r="G90" s="3">
+        <f t="shared" si="14"/>
+        <v>24.034393090575328</v>
+      </c>
+      <c r="H90" s="3">
+        <f t="shared" si="15"/>
+        <v>12.852616625976111</v>
+      </c>
+      <c r="I90" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J90" s="4">
+        <f t="shared" si="17"/>
+        <v>-196.5329009361688</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.87</v>
-      </c>
-      <c r="D90" s="3">
-        <f t="shared" si="10"/>
-        <v>107.96791443850267</v>
-      </c>
-      <c r="E90" s="3">
-        <f t="shared" si="11"/>
-        <v>57.736852640910513</v>
-      </c>
-      <c r="F90" s="3">
-        <f t="shared" si="12"/>
-        <v>30.875322267866583</v>
-      </c>
-      <c r="G90" s="3">
-        <f t="shared" si="13"/>
-        <v>24.034393090575328</v>
-      </c>
-      <c r="H90" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I90" s="4">
-        <f t="shared" si="15"/>
-        <v>-209.38551756214491</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B91" s="3">
         <v>0.88</v>
       </c>
       <c r="C91" s="3">
+        <f t="shared" si="10"/>
+        <v>1.88</v>
+      </c>
+      <c r="D91" s="3">
+        <f t="shared" si="11"/>
+        <v>107.39361702127661</v>
+      </c>
+      <c r="E91" s="3">
+        <f t="shared" si="12"/>
+        <v>57.124264373019471</v>
+      </c>
+      <c r="F91" s="3">
+        <f t="shared" si="13"/>
+        <v>30.385247006925255</v>
+      </c>
+      <c r="G91" s="3">
+        <f t="shared" si="14"/>
+        <v>23.527088656000259</v>
+      </c>
+      <c r="H91" s="3">
+        <f t="shared" si="15"/>
+        <v>12.514408859574607</v>
+      </c>
+      <c r="I91" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J91" s="4">
+        <f t="shared" si="17"/>
+        <v>-199.05537408320382</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.88</v>
-      </c>
-      <c r="D91" s="3">
-        <f t="shared" si="10"/>
-        <v>107.39361702127661</v>
-      </c>
-      <c r="E91" s="3">
-        <f t="shared" si="11"/>
-        <v>57.124264373019471</v>
-      </c>
-      <c r="F91" s="3">
-        <f t="shared" si="12"/>
-        <v>30.385247006925255</v>
-      </c>
-      <c r="G91" s="3">
-        <f t="shared" si="13"/>
-        <v>23.527088656000259</v>
-      </c>
-      <c r="H91" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I91" s="4">
-        <f t="shared" si="15"/>
-        <v>-211.56978294277843</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B92" s="3">
         <v>0.89</v>
       </c>
       <c r="C92" s="3">
+        <f t="shared" si="10"/>
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="D92" s="3">
+        <f t="shared" si="11"/>
+        <v>106.82539682539682</v>
+      </c>
+      <c r="E92" s="3">
+        <f t="shared" si="12"/>
+        <v>56.52137398169144</v>
+      </c>
+      <c r="F92" s="3">
+        <f t="shared" si="13"/>
+        <v>29.905488879201819</v>
+      </c>
+      <c r="G92" s="3">
+        <f t="shared" si="14"/>
+        <v>23.033098740791615</v>
+      </c>
+      <c r="H92" s="3">
+        <f t="shared" si="15"/>
+        <v>12.186824730577573</v>
+      </c>
+      <c r="I92" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J92" s="4">
+        <f t="shared" si="17"/>
+        <v>-201.52781684234074</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.8900000000000001</v>
-      </c>
-      <c r="D92" s="3">
-        <f t="shared" si="10"/>
-        <v>106.82539682539682</v>
-      </c>
-      <c r="E92" s="3">
-        <f t="shared" si="11"/>
-        <v>56.52137398169144</v>
-      </c>
-      <c r="F92" s="3">
-        <f t="shared" si="12"/>
-        <v>29.905488879201819</v>
-      </c>
-      <c r="G92" s="3">
-        <f t="shared" si="13"/>
-        <v>23.033098740791615</v>
-      </c>
-      <c r="H92" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I92" s="4">
-        <f t="shared" si="15"/>
-        <v>-213.71464157291831</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B93" s="3">
         <v>0.9</v>
       </c>
       <c r="C93" s="3">
+        <f t="shared" si="10"/>
+        <v>1.9</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="11"/>
+        <v>106.26315789473685</v>
+      </c>
+      <c r="E93" s="3">
+        <f t="shared" si="12"/>
+        <v>55.927977839335185</v>
+      </c>
+      <c r="F93" s="3">
+        <f t="shared" si="13"/>
+        <v>29.435777810176415</v>
+      </c>
+      <c r="G93" s="3">
+        <f t="shared" si="14"/>
+        <v>22.552006200075198</v>
+      </c>
+      <c r="H93" s="3">
+        <f t="shared" si="15"/>
+        <v>11.869476947407998</v>
+      </c>
+      <c r="I93" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J93" s="4">
+        <f t="shared" si="17"/>
+        <v>-203.95160330826837</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.9</v>
-      </c>
-      <c r="D93" s="3">
-        <f t="shared" si="10"/>
-        <v>106.26315789473685</v>
-      </c>
-      <c r="E93" s="3">
-        <f t="shared" si="11"/>
-        <v>55.927977839335185</v>
-      </c>
-      <c r="F93" s="3">
-        <f t="shared" si="12"/>
-        <v>29.435777810176415</v>
-      </c>
-      <c r="G93" s="3">
-        <f t="shared" si="13"/>
-        <v>22.552006200075198</v>
-      </c>
-      <c r="H93" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I93" s="4">
-        <f t="shared" si="15"/>
-        <v>-215.82108025567638</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B94" s="3">
         <v>0.91</v>
       </c>
       <c r="C94" s="3">
+        <f t="shared" si="10"/>
+        <v>1.9100000000000001</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="11"/>
+        <v>105.70680628272251</v>
+      </c>
+      <c r="E94" s="3">
+        <f t="shared" si="12"/>
+        <v>55.34387763493325</v>
+      </c>
+      <c r="F94" s="3">
+        <f t="shared" si="13"/>
+        <v>28.975852164886515</v>
+      </c>
+      <c r="G94" s="3">
+        <f t="shared" si="14"/>
+        <v>22.083409057047437</v>
+      </c>
+      <c r="H94" s="3">
+        <f t="shared" si="15"/>
+        <v>11.561994270705464</v>
+      </c>
+      <c r="I94" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J94" s="4">
+        <f t="shared" si="17"/>
+        <v>-206.32806058970482</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.9100000000000001</v>
-      </c>
-      <c r="D94" s="3">
-        <f t="shared" si="10"/>
-        <v>105.70680628272251</v>
-      </c>
-      <c r="E94" s="3">
-        <f t="shared" si="11"/>
-        <v>55.34387763493325</v>
-      </c>
-      <c r="F94" s="3">
-        <f t="shared" si="12"/>
-        <v>28.975852164886515</v>
-      </c>
-      <c r="G94" s="3">
-        <f t="shared" si="13"/>
-        <v>22.083409057047437</v>
-      </c>
-      <c r="H94" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I94" s="4">
-        <f t="shared" si="15"/>
-        <v>-217.89005486041029</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B95" s="3">
         <v>0.92</v>
       </c>
       <c r="C95" s="3">
+        <f t="shared" si="10"/>
+        <v>1.92</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="11"/>
+        <v>105.15625</v>
+      </c>
+      <c r="E95" s="3">
+        <f t="shared" si="12"/>
+        <v>54.768880208333336</v>
+      </c>
+      <c r="F95" s="3">
+        <f t="shared" si="13"/>
+        <v>28.525458441840279</v>
+      </c>
+      <c r="G95" s="3">
+        <f t="shared" si="14"/>
+        <v>21.62691987591025</v>
+      </c>
+      <c r="H95" s="3">
+        <f t="shared" si="15"/>
+        <v>11.264020768703256</v>
+      </c>
+      <c r="I95" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J95" s="4">
+        <f t="shared" si="17"/>
+        <v>-208.65847070521286</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.92</v>
-      </c>
-      <c r="D95" s="3">
-        <f t="shared" si="10"/>
-        <v>105.15625</v>
-      </c>
-      <c r="E95" s="3">
-        <f t="shared" si="11"/>
-        <v>54.768880208333336</v>
-      </c>
-      <c r="F95" s="3">
-        <f t="shared" si="12"/>
-        <v>28.525458441840279</v>
-      </c>
-      <c r="G95" s="3">
-        <f t="shared" si="13"/>
-        <v>21.62691987591025</v>
-      </c>
-      <c r="H95" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I95" s="4">
-        <f t="shared" si="15"/>
-        <v>-219.92249147391612</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B96" s="3">
         <v>0.93</v>
       </c>
       <c r="C96" s="3">
+        <f t="shared" si="10"/>
+        <v>1.9300000000000002</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="11"/>
+        <v>104.61139896373057</v>
+      </c>
+      <c r="E96" s="3">
+        <f t="shared" si="12"/>
+        <v>54.202797390533966</v>
+      </c>
+      <c r="F96" s="3">
+        <f t="shared" si="13"/>
+        <v>28.084350979551274</v>
+      </c>
+      <c r="G96" s="3">
+        <f t="shared" si="14"/>
+        <v>21.182165163819665</v>
+      </c>
+      <c r="H96" s="3">
+        <f t="shared" si="15"/>
+        <v>10.97521511078739</v>
+      </c>
+      <c r="I96" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J96" s="4">
+        <f t="shared" si="17"/>
+        <v>-210.94407239157712</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.9300000000000002</v>
-      </c>
-      <c r="D96" s="3">
-        <f t="shared" si="10"/>
-        <v>104.61139896373057</v>
-      </c>
-      <c r="E96" s="3">
-        <f t="shared" si="11"/>
-        <v>54.202797390533966</v>
-      </c>
-      <c r="F96" s="3">
-        <f t="shared" si="12"/>
-        <v>28.084350979551274</v>
-      </c>
-      <c r="G96" s="3">
-        <f t="shared" si="13"/>
-        <v>21.182165163819665</v>
-      </c>
-      <c r="H96" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I96" s="4">
-        <f t="shared" si="15"/>
-        <v>-221.91928750236451</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B97" s="3">
         <v>0.94</v>
       </c>
       <c r="C97" s="3">
+        <f t="shared" si="10"/>
+        <v>1.94</v>
+      </c>
+      <c r="D97" s="3">
+        <f t="shared" si="11"/>
+        <v>104.07216494845362</v>
+      </c>
+      <c r="E97" s="3">
+        <f t="shared" si="12"/>
+        <v>53.645445849718357</v>
+      </c>
+      <c r="F97" s="3">
+        <f t="shared" si="13"/>
+        <v>27.652291675112558</v>
+      </c>
+      <c r="G97" s="3">
+        <f t="shared" si="14"/>
+        <v>20.748784800364525</v>
+      </c>
+      <c r="H97" s="3">
+        <f t="shared" si="15"/>
+        <v>10.695249897095117</v>
+      </c>
+      <c r="I97" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J97" s="4">
+        <f t="shared" si="17"/>
+        <v>-213.18606282925583</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.94</v>
-      </c>
-      <c r="D97" s="3">
-        <f t="shared" si="10"/>
-        <v>104.07216494845362</v>
-      </c>
-      <c r="E97" s="3">
-        <f t="shared" si="11"/>
-        <v>53.645445849718357</v>
-      </c>
-      <c r="F97" s="3">
-        <f t="shared" si="12"/>
-        <v>27.652291675112558</v>
-      </c>
-      <c r="G97" s="3">
-        <f t="shared" si="13"/>
-        <v>20.748784800364525</v>
-      </c>
-      <c r="H97" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I97" s="4">
-        <f t="shared" si="15"/>
-        <v>-223.88131272635096</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B98" s="3">
         <v>0.95</v>
       </c>
       <c r="C98" s="3">
+        <f t="shared" si="10"/>
+        <v>1.95</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="11"/>
+        <v>103.53846153846155</v>
+      </c>
+      <c r="E98" s="3">
+        <f t="shared" si="12"/>
+        <v>53.096646942800795</v>
+      </c>
+      <c r="F98" s="3">
+        <f t="shared" si="13"/>
+        <v>27.229049714256817</v>
+      </c>
+      <c r="G98" s="3">
+        <f t="shared" si="14"/>
+        <v>20.326431493174024</v>
+      </c>
+      <c r="H98" s="3">
+        <f t="shared" si="15"/>
+        <v>10.423811022140525</v>
+      </c>
+      <c r="I98" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J98" s="4">
+        <f t="shared" si="17"/>
+        <v>-215.38559928916629</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.95</v>
-      </c>
-      <c r="D98" s="3">
-        <f t="shared" si="10"/>
-        <v>103.53846153846155</v>
-      </c>
-      <c r="E98" s="3">
-        <f t="shared" si="11"/>
-        <v>53.096646942800795</v>
-      </c>
-      <c r="F98" s="3">
-        <f t="shared" si="12"/>
-        <v>27.229049714256817</v>
-      </c>
-      <c r="G98" s="3">
-        <f t="shared" si="13"/>
-        <v>20.326431493174024</v>
-      </c>
-      <c r="H98" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I98" s="4">
-        <f t="shared" si="15"/>
-        <v>-225.80941031130681</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B99" s="3">
         <v>0.96</v>
       </c>
       <c r="C99" s="3">
+        <f t="shared" si="10"/>
+        <v>1.96</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="11"/>
+        <v>103.01020408163265</v>
+      </c>
+      <c r="E99" s="3">
+        <f t="shared" si="12"/>
+        <v>52.556226572261565</v>
+      </c>
+      <c r="F99" s="3">
+        <f t="shared" si="13"/>
+        <v>26.814401312378347</v>
+      </c>
+      <c r="G99" s="3">
+        <f t="shared" si="14"/>
+        <v>19.914770258331554</v>
+      </c>
+      <c r="H99" s="3">
+        <f t="shared" si="15"/>
+        <v>10.160597070577325</v>
+      </c>
+      <c r="I99" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J99" s="4">
+        <f t="shared" si="17"/>
+        <v>-217.54380070481858</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.96</v>
-      </c>
-      <c r="D99" s="3">
-        <f t="shared" si="10"/>
-        <v>103.01020408163265</v>
-      </c>
-      <c r="E99" s="3">
-        <f t="shared" si="11"/>
-        <v>52.556226572261565</v>
-      </c>
-      <c r="F99" s="3">
-        <f t="shared" si="12"/>
-        <v>26.814401312378347</v>
-      </c>
-      <c r="G99" s="3">
-        <f t="shared" si="13"/>
-        <v>19.914770258331554</v>
-      </c>
-      <c r="H99" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I99" s="4">
-        <f t="shared" si="15"/>
-        <v>-227.7043977753959</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B100" s="3">
         <v>0.97</v>
       </c>
       <c r="C100" s="3">
+        <f t="shared" si="10"/>
+        <v>1.97</v>
+      </c>
+      <c r="D100" s="3">
+        <f t="shared" si="11"/>
+        <v>102.48730964467005</v>
+      </c>
+      <c r="E100" s="3">
+        <f t="shared" si="12"/>
+        <v>52.024015048055865</v>
+      </c>
+      <c r="F100" s="3">
+        <f t="shared" si="13"/>
+        <v>26.408129466018206</v>
+      </c>
+      <c r="G100" s="3">
+        <f t="shared" si="14"/>
+        <v>19.51347792434499</v>
+      </c>
+      <c r="H100" s="3">
+        <f t="shared" si="15"/>
+        <v>9.9053187433223293</v>
+      </c>
+      <c r="I100" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J100" s="4">
+        <f t="shared" si="17"/>
+        <v>-219.66174917358856</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.97</v>
-      </c>
-      <c r="D100" s="3">
-        <f t="shared" si="10"/>
-        <v>102.48730964467005</v>
-      </c>
-      <c r="E100" s="3">
-        <f t="shared" si="11"/>
-        <v>52.024015048055865</v>
-      </c>
-      <c r="F100" s="3">
-        <f t="shared" si="12"/>
-        <v>26.408129466018206</v>
-      </c>
-      <c r="G100" s="3">
-        <f t="shared" si="13"/>
-        <v>19.51347792434499</v>
-      </c>
-      <c r="H100" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I100" s="4">
-        <f t="shared" si="15"/>
-        <v>-229.5670679169109</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B101" s="3">
         <v>0.98</v>
       </c>
       <c r="C101" s="3">
+        <f t="shared" si="10"/>
+        <v>1.98</v>
+      </c>
+      <c r="D101" s="3">
+        <f t="shared" si="11"/>
+        <v>101.96969696969697</v>
+      </c>
+      <c r="E101" s="3">
+        <f t="shared" si="12"/>
+        <v>51.49984695439241</v>
+      </c>
+      <c r="F101" s="3">
+        <f t="shared" si="13"/>
+        <v>26.010023714339603</v>
+      </c>
+      <c r="G101" s="3">
+        <f t="shared" si="14"/>
+        <v>19.122242658492823</v>
+      </c>
+      <c r="H101" s="3">
+        <f t="shared" si="15"/>
+        <v>9.6576983123701137</v>
+      </c>
+      <c r="I101" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J101" s="4">
+        <f t="shared" si="17"/>
+        <v>-221.74049139070806</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.98</v>
-      </c>
-      <c r="D101" s="3">
-        <f t="shared" si="10"/>
-        <v>101.96969696969697</v>
-      </c>
-      <c r="E101" s="3">
-        <f t="shared" si="11"/>
-        <v>51.49984695439241</v>
-      </c>
-      <c r="F101" s="3">
-        <f t="shared" si="12"/>
-        <v>26.010023714339603</v>
-      </c>
-      <c r="G101" s="3">
-        <f t="shared" si="13"/>
-        <v>19.122242658492823</v>
-      </c>
-      <c r="H101" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I101" s="4">
-        <f t="shared" si="15"/>
-        <v>-231.39818970307817</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B102" s="3">
         <v>0.99</v>
       </c>
       <c r="C102" s="3">
+        <f t="shared" si="10"/>
+        <v>1.99</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="11"/>
+        <v>101.45728643216081</v>
+      </c>
+      <c r="E102" s="3">
+        <f t="shared" si="12"/>
+        <v>50.983561021186333</v>
+      </c>
+      <c r="F102" s="3">
+        <f t="shared" si="13"/>
+        <v>25.619879910143887</v>
+      </c>
+      <c r="G102" s="3">
+        <f t="shared" si="14"/>
+        <v>18.740763514430217</v>
+      </c>
+      <c r="H102" s="3">
+        <f t="shared" si="15"/>
+        <v>9.4174691027287523</v>
+      </c>
+      <c r="I102" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J102" s="4">
+        <f t="shared" si="17"/>
+        <v>-223.78104001935</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="str">
         <f t="shared" si="9"/>
-        <v>1.99</v>
-      </c>
-      <c r="D102" s="3">
-        <f t="shared" si="10"/>
-        <v>101.45728643216081</v>
-      </c>
-      <c r="E102" s="3">
-        <f t="shared" si="11"/>
-        <v>50.983561021186333</v>
-      </c>
-      <c r="F102" s="3">
-        <f t="shared" si="12"/>
-        <v>25.619879910143887</v>
-      </c>
-      <c r="G102" s="3">
-        <f t="shared" si="13"/>
-        <v>18.740763514430217</v>
-      </c>
-      <c r="H102" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I102" s="4">
-        <f t="shared" si="15"/>
-        <v>-233.19850912207875</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="6" t="str">
-        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="B103" s="3">
         <v>1</v>
       </c>
       <c r="C103" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="D103" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>100.95</v>
       </c>
       <c r="E103" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>50.475000000000001</v>
       </c>
       <c r="F103" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>25.237500000000001</v>
       </c>
       <c r="G103" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18.368749999999999</v>
       </c>
       <c r="H103" s="3">
-        <f t="shared" si="14"/>
-        <v>-430</v>
-      </c>
-      <c r="I103" s="4">
         <f t="shared" si="15"/>
-        <v>-234.96874999999997</v>
+        <v>9.1843749999999993</v>
+      </c>
+      <c r="I103" s="3">
+        <f t="shared" si="16"/>
+        <v>-430</v>
+      </c>
+      <c r="J103" s="4">
+        <f t="shared" si="17"/>
+        <v>-225.78437499999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>